<commit_message>
duplicate lookup with _ref
</commit_message>
<xml_diff>
--- a/Attributes and Objects Documentation.xlsx
+++ b/Attributes and Objects Documentation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\tahoe\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{605D53E4-EB06-402D-905F-24E712AFBED2}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5E8C247-0E77-427E-AA2B-F34B1368EF58}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{11D50969-177D-481F-A7AD-9647F67FC210}"/>
   </bookViews>
@@ -16,6 +16,7 @@
     <sheet name="current" sheetId="2" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
     <sheet name="misp" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet2" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1045" uniqueCount="561">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1430" uniqueCount="583">
   <si>
     <t xml:space="preserve">md5 </t>
   </si>
@@ -1659,9 +1660,6 @@
     <t>filename</t>
   </si>
   <si>
-    <t>alias</t>
-  </si>
-  <si>
     <t>tahoe object</t>
   </si>
   <si>
@@ -1712,9 +1710,6 @@
   </si>
   <si>
     <t>cryptocurrency_address</t>
-  </si>
-  <si>
-    <t>cve</t>
   </si>
   <si>
     <t>if [:3] == "CVE": cve_id</t>
@@ -1791,6 +1786,81 @@
   </si>
   <si>
     <t>location</t>
+  </si>
+  <si>
+    <t>memory</t>
+  </si>
+  <si>
+    <t>pattern_in_memory
+data</t>
+  </si>
+  <si>
+    <t>traffic</t>
+  </si>
+  <si>
+    <t>pattern_in_traffic
+data</t>
+  </si>
+  <si>
+    <t>named_pipe</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>body</t>
+  </si>
+  <si>
+    <t>prtn
+phone</t>
+  </si>
+  <si>
+    <t>dns_soa_email</t>
+  </si>
+  <si>
+    <t>email_reply_to</t>
+  </si>
+  <si>
+    <t>statement_of_authority</t>
+  </si>
+  <si>
+    <t>dns</t>
+  </si>
+  <si>
+    <t>hex_data</t>
+  </si>
+  <si>
+    <t>jabber_id</t>
+  </si>
+  <si>
+    <t>twitter_id</t>
+  </si>
+  <si>
+    <t>twitter</t>
+  </si>
+  <si>
+    <t>bytes</t>
+  </si>
+  <si>
+    <t>size_in_bytes</t>
+  </si>
+  <si>
+    <t>mime_boundary</t>
+  </si>
+  <si>
+    <t>reply_to</t>
+  </si>
+  <si>
+    <t>message_id</t>
+  </si>
+  <si>
+    <t>x_mailer</t>
+  </si>
+  <si>
+    <t>tahoe alias</t>
+  </si>
+  <si>
+    <t>misp alias</t>
   </si>
 </sst>
 </file>
@@ -2043,7 +2113,21 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="4">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -2696,8 +2780,8 @@
   <dimension ref="A1:G163"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A122" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D132" sqref="D132"/>
+      <pane ySplit="1" topLeftCell="A116" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A123" sqref="A123"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5182,7 +5266,7 @@
     <sortCondition ref="D1"/>
   </sortState>
   <conditionalFormatting sqref="A8:E8 A1:D7 F1:F7 F9:F1048576 G1:XFD1048576 E1:E1048576 A9:D1048576">
-    <cfRule type="expression" dxfId="1" priority="1">
+    <cfRule type="expression" dxfId="2" priority="1">
       <formula>MOD(ROW()/2,1)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5193,1331 +5277,2833 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FD3A4BA-035A-49B6-AE8D-CE931CE2DC31}">
-  <dimension ref="A1:E159"/>
+  <dimension ref="A1:F159"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A48" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D73" sqref="D73"/>
+      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" thickBottom="1" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="37.88671875" style="28" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.44140625" style="28" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.77734375" style="28" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.44140625" style="28" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.88671875" style="28"/>
+    <col min="2" max="2" width="22.88671875" style="28" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.33203125" style="28" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.21875" style="28" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.5546875" style="28" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.109375" style="28" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.88671875" style="28"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="27" customFormat="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" s="27" customFormat="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="27" t="s">
         <v>315</v>
       </c>
       <c r="B1" s="27" t="s">
+        <v>582</v>
+      </c>
+      <c r="C1" s="27" t="s">
         <v>519</v>
       </c>
-      <c r="C1" s="27" t="s">
+      <c r="D1" s="27" t="s">
+        <v>581</v>
+      </c>
+      <c r="E1" s="27" t="s">
         <v>521</v>
       </c>
-      <c r="D1" s="27" t="s">
-        <v>522</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" thickBot="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="28" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="3" spans="1:4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="28" t="s">
         <v>311</v>
       </c>
     </row>
-    <row r="4" spans="1:4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="28" t="s">
         <v>54</v>
       </c>
-      <c r="B4" s="28" t="s">
+      <c r="C4" s="28" t="s">
         <v>325</v>
       </c>
-      <c r="C4" s="28" t="s">
-        <v>543</v>
-      </c>
       <c r="D4" s="28" t="s">
+        <v>541</v>
+      </c>
+      <c r="E4" s="28" t="s">
         <v>345</v>
       </c>
     </row>
-    <row r="5" spans="1:4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="28" t="s">
         <v>84</v>
       </c>
-      <c r="B5" s="28" t="s">
+      <c r="C5" s="28" t="s">
         <v>520</v>
       </c>
-      <c r="D5" s="28" t="s">
+      <c r="E5" s="28" t="s">
         <v>374</v>
       </c>
     </row>
-    <row r="6" spans="1:4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="28" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="7" spans="1:4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="28" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="8" spans="1:4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="28" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="9" spans="1:4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="28" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="10" spans="1:4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="28" t="s">
         <v>309</v>
       </c>
     </row>
-    <row r="11" spans="1:4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="28" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="12" spans="1:4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="28" t="s">
         <v>113</v>
       </c>
-      <c r="B12" s="28" t="s">
+      <c r="C12" s="28" t="s">
+        <v>536</v>
+      </c>
+      <c r="D12" s="28" t="s">
         <v>537</v>
       </c>
-      <c r="C12" s="28" t="s">
-        <v>538</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" thickBot="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="13" spans="1:5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="28" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B13" s="28" t="s">
+        <v>319</v>
+      </c>
+      <c r="C13" s="28" t="s">
+        <v>564</v>
+      </c>
+      <c r="E13" s="28" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="28" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B14" s="28" t="s">
+        <v>320</v>
+      </c>
+      <c r="C14" s="28" t="s">
+        <v>524</v>
+      </c>
+      <c r="E14" s="28" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="28" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="16" spans="1:4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="28" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="17" spans="1:5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="28" t="s">
         <v>89</v>
       </c>
-      <c r="B17" s="28" t="s">
+      <c r="C17" s="28" t="s">
         <v>340</v>
       </c>
-      <c r="C17" s="28" t="s">
+      <c r="D17" s="28" t="s">
         <v>353</v>
       </c>
     </row>
-    <row r="18" spans="1:5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="28" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="19" spans="1:5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="28" t="s">
         <v>307</v>
       </c>
     </row>
-    <row r="20" spans="1:5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="28" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="21" spans="1:5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="28" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="22" spans="1:5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="28" t="s">
         <v>219</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C22" s="28" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="28" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="24" spans="1:5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="28" t="s">
         <v>217</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C24" s="28" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="28" t="s">
         <v>212</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B25" s="28" t="s">
+        <v>567</v>
+      </c>
+      <c r="C25" s="28" t="s">
+        <v>362</v>
+      </c>
+      <c r="E25" s="28" t="s">
+        <v>569</v>
+      </c>
+      <c r="F25" s="28" t="s">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="28" t="s">
         <v>22</v>
       </c>
-      <c r="B26" s="28" t="s">
+      <c r="C26" s="28" t="s">
         <v>344</v>
       </c>
     </row>
-    <row r="27" spans="1:5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="B27" s="28" t="s">
-        <v>541</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C27" s="28" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" s="28" t="s">
         <v>32</v>
       </c>
       <c r="B28" s="28" t="s">
+        <v>545</v>
+      </c>
+      <c r="C28" s="28" t="s">
         <v>520</v>
       </c>
-      <c r="C28" s="28" t="s">
-        <v>547</v>
-      </c>
-      <c r="D28" s="28" t="s">
-        <v>544</v>
-      </c>
       <c r="E28" s="28" t="s">
+        <v>542</v>
+      </c>
+      <c r="F28" s="28" t="s">
         <v>368</v>
       </c>
     </row>
-    <row r="29" spans="1:5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" s="28" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B29" s="28" t="s">
+        <v>321</v>
+      </c>
+      <c r="C29" s="28" t="s">
+        <v>426</v>
+      </c>
+      <c r="E29" s="28" t="s">
+        <v>565</v>
+      </c>
+      <c r="F29" s="28" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="B30" s="28" t="s">
+      <c r="C30" s="28" t="s">
         <v>362</v>
       </c>
-      <c r="D30" s="28" t="s">
+      <c r="E30" s="28" t="s">
         <v>363</v>
       </c>
-      <c r="E30" s="28" t="s">
+      <c r="F30" s="28" t="s">
         <v>368</v>
       </c>
     </row>
-    <row r="31" spans="1:5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A31" s="28" t="s">
         <v>233</v>
       </c>
-      <c r="B31" s="28" t="s">
+      <c r="C31" s="28" t="s">
         <v>365</v>
       </c>
-      <c r="D31" s="28" t="s">
+      <c r="E31" s="28" t="s">
         <v>363</v>
       </c>
-      <c r="E31" s="28" t="s">
+      <c r="F31" s="28" t="s">
         <v>368</v>
       </c>
     </row>
-    <row r="32" spans="1:5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" s="28" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="33" spans="1:5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A33" s="28" t="s">
         <v>247</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C33" s="28" t="s">
+        <v>579</v>
+      </c>
+      <c r="E33" s="28" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A34" s="28" t="s">
         <v>243</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C34" s="28" t="s">
+        <v>577</v>
+      </c>
+      <c r="E34" s="28" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A35" s="28" t="s">
         <v>239</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B35" s="28" t="s">
+        <v>568</v>
+      </c>
+      <c r="C35" s="28" t="s">
+        <v>362</v>
+      </c>
+      <c r="E35" s="28" t="s">
+        <v>578</v>
+      </c>
+      <c r="F35" s="28" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A36" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="B36" s="28" t="s">
+      <c r="C36" s="28" t="s">
         <v>362</v>
       </c>
-      <c r="D36" s="28" t="s">
+      <c r="E36" s="28" t="s">
         <v>367</v>
       </c>
-      <c r="E36" s="28" t="s">
+      <c r="F36" s="28" t="s">
         <v>368</v>
       </c>
     </row>
-    <row r="37" spans="1:5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A37" s="28" t="s">
         <v>235</v>
       </c>
-      <c r="B37" s="28" t="s">
+      <c r="C37" s="28" t="s">
         <v>365</v>
       </c>
-      <c r="D37" s="28" t="s">
+      <c r="E37" s="28" t="s">
         <v>367</v>
       </c>
-      <c r="E37" s="28" t="s">
+      <c r="F37" s="28" t="s">
         <v>368</v>
       </c>
     </row>
-    <row r="38" spans="1:5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A38" s="28" t="s">
         <v>30</v>
       </c>
-      <c r="B38" s="28" t="s">
-        <v>530</v>
-      </c>
-      <c r="D38" s="28" t="s">
+      <c r="C38" s="28" t="s">
+        <v>529</v>
+      </c>
+      <c r="E38" s="28" t="s">
         <v>368</v>
       </c>
     </row>
-    <row r="39" spans="1:5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A39" s="28" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="40" spans="1:5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A40" s="28" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="41" spans="1:5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C40" s="28" t="s">
+        <v>580</v>
+      </c>
+      <c r="E40" s="28" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A41" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="B41" s="28" t="s">
+      <c r="C41" s="28" t="s">
         <v>520</v>
       </c>
-      <c r="D41" s="28" t="s">
+      <c r="E41" s="28" t="s">
         <v>374</v>
       </c>
     </row>
-    <row r="42" spans="1:5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A42" s="28" t="s">
         <v>166</v>
       </c>
-      <c r="B42" s="28" t="s">
+      <c r="C42" s="28" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="43" spans="1:5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A43" s="28" t="s">
         <v>172</v>
       </c>
-      <c r="B43" s="28" t="s">
+      <c r="C43" s="28" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="44" spans="1:5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A44" s="28" t="s">
         <v>170</v>
       </c>
-      <c r="B44" s="28" t="s">
+      <c r="C44" s="28" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="45" spans="1:5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A45" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="B45" s="28" t="s">
+      <c r="C45" s="28" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="46" spans="1:5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A46" s="28" t="s">
         <v>174</v>
       </c>
-      <c r="B46" s="28" t="s">
+      <c r="C46" s="28" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="47" spans="1:5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A47" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="B47" s="28" t="s">
+      <c r="C47" s="28" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="48" spans="1:5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A48" s="28" t="s">
         <v>176</v>
       </c>
-      <c r="B48" s="28" t="s">
+      <c r="C48" s="28" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="49" spans="1:3" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A49" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="B49" s="28" t="s">
+      <c r="C49" s="28" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="50" spans="1:3" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A50" s="28" t="s">
         <v>178</v>
       </c>
-      <c r="B50" s="28" t="s">
+      <c r="C50" s="28" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="51" spans="1:3" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A51" s="28" t="s">
         <v>180</v>
       </c>
-      <c r="B51" s="28" t="s">
+      <c r="C51" s="28" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="52" spans="1:3" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A52" s="28" t="s">
         <v>182</v>
       </c>
-      <c r="B52" s="28" t="s">
+      <c r="C52" s="28" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="53" spans="1:3" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A53" s="28" t="s">
         <v>184</v>
       </c>
-      <c r="B53" s="28" t="s">
+      <c r="C53" s="28" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="54" spans="1:3" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A54" s="28" t="s">
         <v>168</v>
       </c>
-      <c r="B54" s="28" t="s">
+      <c r="C54" s="28" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="55" spans="1:3" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A55" s="28" t="s">
         <v>186</v>
       </c>
-      <c r="B55" s="28" t="s">
+      <c r="C55" s="28" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="56" spans="1:3" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A56" s="28" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="57" spans="1:3" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A57" s="28" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="58" spans="1:3" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A58" s="28" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="59" spans="1:3" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A59" s="28" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="60" spans="1:3" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A60" s="28" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="61" spans="1:3" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A61" s="28" t="s">
         <v>253</v>
       </c>
-      <c r="B61" s="28" t="s">
+      <c r="C61" s="28" t="s">
         <v>513</v>
       </c>
-      <c r="C61" s="28" t="s">
+      <c r="D61" s="28" t="s">
         <v>381</v>
       </c>
     </row>
-    <row r="62" spans="1:3" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A62" s="28" t="s">
         <v>251</v>
       </c>
-      <c r="B62" s="28" t="s">
-        <v>542</v>
-      </c>
       <c r="C62" s="28" t="s">
+        <v>540</v>
+      </c>
+      <c r="D62" s="28" t="s">
         <v>381</v>
       </c>
     </row>
-    <row r="63" spans="1:3" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A63" s="28" t="s">
         <v>249</v>
       </c>
-      <c r="B63" s="28" t="s">
+      <c r="C63" s="28" t="s">
         <v>452</v>
       </c>
-      <c r="C63" s="28" t="s">
+      <c r="D63" s="28" t="s">
         <v>381</v>
       </c>
     </row>
-    <row r="64" spans="1:3" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A64" s="28" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="65" spans="1:4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A65" s="28" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="66" spans="1:4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A66" s="28" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="67" spans="1:4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C66" s="28" t="s">
+        <v>571</v>
+      </c>
+      <c r="D66" s="28" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A67" s="28" t="s">
         <v>20</v>
       </c>
-      <c r="B67" s="28" t="s">
+      <c r="C67" s="28" t="s">
         <v>389</v>
       </c>
     </row>
-    <row r="68" spans="1:4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A68" s="28" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="69" spans="1:4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A69" s="28" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="70" spans="1:4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A70" s="28" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="71" spans="1:4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A71" s="28" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="72" spans="1:4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A72" s="28" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="73" spans="1:4" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:5" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A73" s="28" t="s">
         <v>146</v>
       </c>
-      <c r="B73" s="28" t="s">
+      <c r="C73" s="28" t="s">
         <v>396</v>
       </c>
-      <c r="C73" s="29" t="s">
-        <v>528</v>
-      </c>
-      <c r="D73" s="28" t="s">
+      <c r="D73" s="29" t="s">
+        <v>527</v>
+      </c>
+      <c r="E73" s="28" t="s">
         <v>374</v>
       </c>
     </row>
-    <row r="74" spans="1:4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A74" s="28" t="s">
         <v>18</v>
       </c>
-      <c r="B74" s="28" t="s">
+      <c r="C74" s="28" t="s">
         <v>499</v>
       </c>
-      <c r="C74" s="28" t="s">
-        <v>524</v>
-      </c>
       <c r="D74" s="28" t="s">
+        <v>523</v>
+      </c>
+      <c r="E74" s="28" t="s">
         <v>363</v>
       </c>
     </row>
-    <row r="75" spans="1:4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A75" s="28" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="76" spans="1:4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A76" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="B76" s="28" t="s">
+      <c r="C76" s="28" t="s">
         <v>499</v>
       </c>
-      <c r="C76" s="28" t="s">
-        <v>524</v>
-      </c>
       <c r="D76" s="28" t="s">
+        <v>523</v>
+      </c>
+      <c r="E76" s="28" t="s">
         <v>367</v>
       </c>
     </row>
-    <row r="77" spans="1:4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A77" s="28" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="78" spans="1:4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A78" s="28" t="s">
         <v>283</v>
       </c>
     </row>
-    <row r="79" spans="1:4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A79" s="28" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="80" spans="1:4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A80" s="28" t="s">
         <v>255</v>
       </c>
-    </row>
-    <row r="81" spans="1:4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C80" s="28" t="s">
+        <v>452</v>
+      </c>
+      <c r="D80" s="28" t="s">
+        <v>572</v>
+      </c>
+      <c r="E80" s="28" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A81" s="28" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="82" spans="1:4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A82" s="28" t="s">
         <v>87</v>
       </c>
-      <c r="B82" s="28" t="s">
+      <c r="C82" s="28" t="s">
         <v>39</v>
       </c>
-      <c r="C82" s="28" t="s">
+      <c r="D82" s="28" t="s">
         <v>461</v>
       </c>
-      <c r="D82" s="28" t="s">
-        <v>529</v>
-      </c>
-    </row>
-    <row r="83" spans="1:4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E82" s="28" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A83" s="28" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="84" spans="1:4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A84" s="28" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="85" spans="1:4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A85" s="28" t="s">
         <v>86</v>
       </c>
-      <c r="B85" s="28" t="s">
+      <c r="C85" s="28" t="s">
         <v>484</v>
       </c>
-      <c r="D85" s="28" t="s">
+      <c r="E85" s="28" t="s">
         <v>407</v>
       </c>
     </row>
-    <row r="86" spans="1:4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A86" s="28" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="87" spans="1:4" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:5" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A87" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="B87" s="28" t="s">
+      <c r="C87" s="28" t="s">
         <v>408</v>
       </c>
-      <c r="C87" s="29" t="s">
-        <v>528</v>
-      </c>
-    </row>
-    <row r="88" spans="1:4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D87" s="29" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A88" s="28" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="89" spans="1:4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A89" s="28" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="90" spans="1:4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A90" s="28" t="s">
         <v>305</v>
       </c>
-      <c r="B90" s="28" t="s">
+      <c r="C90" s="28" t="s">
         <v>413</v>
       </c>
-      <c r="D90" s="28" t="s">
+      <c r="E90" s="28" t="s">
         <v>414</v>
       </c>
     </row>
-    <row r="91" spans="1:4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A91" s="28" t="s">
         <v>99</v>
       </c>
-      <c r="B91" s="28" t="s">
+      <c r="C91" s="28" t="s">
         <v>415</v>
       </c>
     </row>
-    <row r="92" spans="1:4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A92" s="28" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="93" spans="1:4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C92" s="28" t="s">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A93" s="28" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="94" spans="1:4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A94" s="28" t="s">
         <v>95</v>
       </c>
-      <c r="B94" s="28" t="s">
+      <c r="C94" s="28" t="s">
         <v>418</v>
       </c>
     </row>
-    <row r="95" spans="1:4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A95" s="28" t="s">
         <v>303</v>
       </c>
     </row>
-    <row r="96" spans="1:4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A96" s="28" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="97" spans="1:4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A97" s="28" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="98" spans="1:4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A98" s="28" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="99" spans="1:4" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:5" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A99" s="28" t="s">
         <v>62</v>
       </c>
-      <c r="B99" s="28" t="s">
-        <v>548</v>
-      </c>
-      <c r="C99" s="29" t="s">
-        <v>549</v>
-      </c>
-      <c r="D99" s="28" t="s">
+      <c r="C99" s="28" t="s">
+        <v>546</v>
+      </c>
+      <c r="D99" s="29" t="s">
+        <v>547</v>
+      </c>
+      <c r="E99" s="28" t="s">
         <v>374</v>
       </c>
     </row>
-    <row r="100" spans="1:4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:5" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A100" s="28" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="101" spans="1:4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C100" s="28" t="s">
+        <v>546</v>
+      </c>
+      <c r="D100" s="29" t="s">
+        <v>560</v>
+      </c>
+      <c r="E100" s="28" t="s">
+        <v>559</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A101" s="28" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="102" spans="1:4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C101" s="28" t="s">
+        <v>546</v>
+      </c>
+      <c r="D101" s="29" t="s">
+        <v>562</v>
+      </c>
+      <c r="E101" s="28" t="s">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A102" s="28" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="103" spans="1:4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A103" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="B103" s="28" t="s">
-        <v>545</v>
-      </c>
       <c r="C103" s="28" t="s">
+        <v>543</v>
+      </c>
+      <c r="D103" s="28" t="s">
         <v>432</v>
       </c>
-      <c r="D103" s="28" t="s">
+      <c r="E103" s="28" t="s">
         <v>374</v>
       </c>
     </row>
-    <row r="104" spans="1:4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:5" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A104" s="28" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="105" spans="1:4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C104" s="28" t="s">
+        <v>435</v>
+      </c>
+      <c r="D104" s="29" t="s">
+        <v>527</v>
+      </c>
+      <c r="E104" s="28" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A105" s="28" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="106" spans="1:4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C105" s="28" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A106" s="28" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="107" spans="1:4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A107" s="28" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="108" spans="1:4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A108" s="28" t="s">
         <v>301</v>
       </c>
     </row>
-    <row r="109" spans="1:4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A109" s="28" t="s">
         <v>297</v>
       </c>
     </row>
-    <row r="110" spans="1:4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A110" s="28" t="s">
         <v>221</v>
       </c>
-      <c r="B110" s="28" t="s">
+      <c r="C110" s="28" t="s">
         <v>440</v>
       </c>
     </row>
-    <row r="111" spans="1:4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A111" s="28" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="112" spans="1:4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:5" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A112" s="28" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="113" spans="1:4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C112" s="28" t="s">
+        <v>442</v>
+      </c>
+      <c r="D112" s="29" t="s">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A113" s="28" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="114" spans="1:4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A114" s="28" t="s">
         <v>50</v>
       </c>
-      <c r="B114" s="28" t="s">
+      <c r="C114" s="28" t="s">
         <v>443</v>
       </c>
-      <c r="D114" s="28" t="s">
+      <c r="E114" s="28" t="s">
         <v>444</v>
       </c>
     </row>
-    <row r="115" spans="1:4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A115" s="28" t="s">
         <v>52</v>
       </c>
-      <c r="B115" s="28" t="s">
+      <c r="C115" s="28" t="s">
         <v>493</v>
       </c>
-      <c r="D115" s="28" t="s">
+      <c r="E115" s="28" t="s">
         <v>444</v>
       </c>
     </row>
-    <row r="116" spans="1:4" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:5" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A116" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="B116" s="28" t="s">
-        <v>526</v>
-      </c>
-      <c r="C116" s="29" t="s">
-        <v>528</v>
-      </c>
-    </row>
-    <row r="117" spans="1:4" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C116" s="28" t="s">
+        <v>525</v>
+      </c>
+      <c r="D116" s="29" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A117" s="28" t="s">
         <v>152</v>
       </c>
-      <c r="B117" s="28" t="s">
+      <c r="C117" s="28" t="s">
+        <v>526</v>
+      </c>
+      <c r="D117" s="29" t="s">
         <v>527</v>
       </c>
-      <c r="C117" s="29" t="s">
-        <v>528</v>
-      </c>
-    </row>
-    <row r="118" spans="1:4" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="118" spans="1:5" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A118" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="B118" s="28" t="s">
-        <v>523</v>
-      </c>
-      <c r="C118" s="29" t="s">
-        <v>528</v>
-      </c>
-    </row>
-    <row r="119" spans="1:4" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C118" s="28" t="s">
+        <v>522</v>
+      </c>
+      <c r="D118" s="29" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A119" s="28" t="s">
         <v>154</v>
       </c>
-      <c r="B119" s="28" t="s">
+      <c r="C119" s="28" t="s">
         <v>154</v>
       </c>
-      <c r="C119" s="29" t="s">
-        <v>528</v>
-      </c>
-    </row>
-    <row r="120" spans="1:4" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D119" s="29" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A120" s="28" t="s">
         <v>156</v>
       </c>
-      <c r="B120" s="28" t="s">
+      <c r="C120" s="28" t="s">
         <v>156</v>
       </c>
-      <c r="C120" s="29" t="s">
-        <v>528</v>
-      </c>
-    </row>
-    <row r="121" spans="1:4" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D120" s="29" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A121" s="28" t="s">
         <v>158</v>
       </c>
-      <c r="B121" s="28" t="s">
+      <c r="C121" s="28" t="s">
         <v>158</v>
       </c>
-      <c r="C121" s="29" t="s">
-        <v>528</v>
-      </c>
-    </row>
-    <row r="122" spans="1:4" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D121" s="29" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A122" s="28" t="s">
         <v>160</v>
       </c>
-      <c r="B122" s="28" t="s">
+      <c r="C122" s="28" t="s">
         <v>160</v>
       </c>
-      <c r="C122" s="29" t="s">
-        <v>528</v>
-      </c>
-    </row>
-    <row r="123" spans="1:4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D122" s="29" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A123" s="28" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="124" spans="1:4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C123" s="28" t="s">
+        <v>446</v>
+      </c>
+      <c r="E123" s="28" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A124" s="28" t="s">
         <v>213</v>
       </c>
-    </row>
-    <row r="125" spans="1:4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C124" s="28" t="s">
+        <v>575</v>
+      </c>
+      <c r="D124" s="28" t="s">
+        <v>576</v>
+      </c>
+      <c r="E124" s="28" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A125" s="28" t="s">
         <v>56</v>
       </c>
-      <c r="B125" s="28" t="s">
+      <c r="C125" s="28" t="s">
         <v>449</v>
       </c>
-      <c r="C125" s="29" t="s">
-        <v>546</v>
-      </c>
-      <c r="D125" s="28" t="s">
+      <c r="D125" s="29" t="s">
+        <v>544</v>
+      </c>
+      <c r="E125" s="28" t="s">
         <v>355</v>
       </c>
     </row>
-    <row r="126" spans="1:4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A126" s="28" t="s">
         <v>289</v>
       </c>
     </row>
-    <row r="127" spans="1:4" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:5" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A127" s="28" t="s">
         <v>144</v>
       </c>
-      <c r="B127" s="28" t="s">
+      <c r="C127" s="28" t="s">
         <v>450</v>
       </c>
-      <c r="C127" s="29" t="s">
-        <v>528</v>
-      </c>
-    </row>
-    <row r="128" spans="1:4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D127" s="29" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A128" s="28" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="129" spans="1:5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A129" s="28" t="s">
         <v>103</v>
       </c>
-      <c r="B129" s="28" t="s">
+      <c r="C129" s="28" t="s">
         <v>362</v>
       </c>
-      <c r="D129" s="28" t="s">
+      <c r="E129" s="28" t="s">
         <v>451</v>
       </c>
     </row>
-    <row r="130" spans="1:5" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:6" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A130" s="28" t="s">
         <v>111</v>
       </c>
-      <c r="B130" s="28" t="s">
-        <v>556</v>
-      </c>
-      <c r="C130" s="29" t="s">
-        <v>557</v>
-      </c>
-      <c r="D130" s="28" t="s">
+      <c r="C130" s="28" t="s">
+        <v>554</v>
+      </c>
+      <c r="D130" s="29" t="s">
+        <v>555</v>
+      </c>
+      <c r="E130" s="28" t="s">
         <v>451</v>
       </c>
     </row>
-    <row r="131" spans="1:5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A131" s="28" t="s">
         <v>109</v>
       </c>
-      <c r="B131" s="28" t="s">
-        <v>560</v>
-      </c>
       <c r="C131" s="28" t="s">
+        <v>558</v>
+      </c>
+      <c r="D131" s="28" t="s">
         <v>455</v>
       </c>
-      <c r="D131" s="28" t="s">
+      <c r="E131" s="28" t="s">
         <v>451</v>
       </c>
     </row>
-    <row r="132" spans="1:5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A132" s="28" t="s">
         <v>105</v>
       </c>
-      <c r="B132" s="28" t="s">
+      <c r="C132" s="28" t="s">
         <v>454</v>
       </c>
-      <c r="D132" s="28" t="s">
+      <c r="E132" s="28" t="s">
         <v>451</v>
       </c>
     </row>
-    <row r="133" spans="1:5" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:6" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A133" s="28" t="s">
         <v>107</v>
       </c>
-      <c r="B133" s="28" t="s">
-        <v>525</v>
-      </c>
-      <c r="C133" s="29" t="s">
-        <v>558</v>
-      </c>
-      <c r="D133" s="28" t="s">
+      <c r="C133" s="28" t="s">
+        <v>524</v>
+      </c>
+      <c r="D133" s="29" t="s">
+        <v>556</v>
+      </c>
+      <c r="E133" s="28" t="s">
         <v>513</v>
       </c>
-      <c r="E133" s="28" t="s">
+      <c r="F133" s="28" t="s">
         <v>451</v>
       </c>
     </row>
-    <row r="134" spans="1:5" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:6" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A134" s="28" t="s">
         <v>101</v>
       </c>
-      <c r="B134" s="28" t="s">
-        <v>525</v>
-      </c>
-      <c r="C134" s="29" t="s">
-        <v>559</v>
-      </c>
-      <c r="D134" s="28" t="s">
-        <v>551</v>
+      <c r="C134" s="28" t="s">
+        <v>524</v>
+      </c>
+      <c r="D134" s="29" t="s">
+        <v>557</v>
       </c>
       <c r="E134" s="28" t="s">
+        <v>549</v>
+      </c>
+      <c r="F134" s="28" t="s">
         <v>451</v>
       </c>
     </row>
-    <row r="135" spans="1:5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A135" s="28" t="s">
         <v>91</v>
       </c>
-      <c r="B135" s="28" t="s">
+      <c r="C135" s="28" t="s">
         <v>353</v>
       </c>
     </row>
-    <row r="136" spans="1:5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A136" s="28" t="s">
         <v>133</v>
       </c>
-      <c r="B136" s="28" t="s">
-        <v>525</v>
-      </c>
       <c r="C136" s="28" t="s">
-        <v>550</v>
+        <v>524</v>
       </c>
       <c r="D136" s="28" t="s">
+        <v>548</v>
+      </c>
+      <c r="E136" s="28" t="s">
         <v>457</v>
       </c>
     </row>
-    <row r="137" spans="1:5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A137" s="28" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="138" spans="1:5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A138" s="28" t="s">
         <v>293</v>
       </c>
     </row>
-    <row r="139" spans="1:5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A139" s="28" t="s">
         <v>257</v>
       </c>
-    </row>
-    <row r="140" spans="1:5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C139" s="28" t="s">
+        <v>452</v>
+      </c>
+      <c r="D139" s="28" t="s">
+        <v>573</v>
+      </c>
+      <c r="E139" s="28" t="s">
+        <v>574</v>
+      </c>
+    </row>
+    <row r="140" spans="1:6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A140" s="28" t="s">
         <v>140</v>
       </c>
-      <c r="B140" s="28" t="s">
+      <c r="C140" s="28" t="s">
         <v>461</v>
       </c>
     </row>
-    <row r="141" spans="1:5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A141" s="28" t="s">
         <v>38</v>
       </c>
-      <c r="B141" s="28" t="s">
+      <c r="C141" s="28" t="s">
         <v>39</v>
       </c>
-      <c r="C141" s="28" t="s">
+      <c r="D141" s="28" t="s">
         <v>461</v>
       </c>
     </row>
-    <row r="142" spans="1:5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A142" s="28" t="s">
         <v>42</v>
       </c>
-      <c r="B142" s="28" t="s">
+      <c r="C142" s="28" t="s">
         <v>479</v>
       </c>
-      <c r="C142" s="28" t="s">
-        <v>552</v>
-      </c>
       <c r="D142" s="28" t="s">
+        <v>550</v>
+      </c>
+      <c r="E142" s="28" t="s">
         <v>392</v>
       </c>
     </row>
-    <row r="143" spans="1:5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A143" s="28" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="144" spans="1:5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A144" s="28" t="s">
         <v>82</v>
       </c>
-      <c r="B144" s="28" t="s">
-        <v>540</v>
-      </c>
       <c r="C144" s="28" t="s">
+        <v>538</v>
+      </c>
+      <c r="D144" s="28" t="s">
         <v>478</v>
       </c>
-      <c r="D144" s="28" t="s">
-        <v>539</v>
-      </c>
-    </row>
-    <row r="145" spans="1:5" thickBot="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="145" spans="1:6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A145" s="28" t="s">
         <v>204</v>
       </c>
-      <c r="B145" s="28" t="s">
+      <c r="C145" s="28" t="s">
+        <v>530</v>
+      </c>
+      <c r="D145" s="28" t="s">
         <v>531</v>
       </c>
-      <c r="C145" s="28" t="s">
-        <v>532</v>
-      </c>
-      <c r="D145" s="28" t="s">
+      <c r="E145" s="28" t="s">
         <v>476</v>
       </c>
     </row>
-    <row r="146" spans="1:5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A146" s="28" t="s">
         <v>194</v>
       </c>
-      <c r="B146" s="28" t="s">
+      <c r="C146" s="28" t="s">
         <v>362</v>
       </c>
-      <c r="D146" s="28" t="s">
-        <v>535</v>
-      </c>
       <c r="E146" s="28" t="s">
+        <v>534</v>
+      </c>
+      <c r="F146" s="28" t="s">
         <v>476</v>
       </c>
     </row>
-    <row r="147" spans="1:5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A147" s="28" t="s">
         <v>198</v>
       </c>
-      <c r="B147" s="28" t="s">
-        <v>525</v>
-      </c>
-      <c r="D147" s="28" t="s">
-        <v>535</v>
+      <c r="C147" s="28" t="s">
+        <v>524</v>
       </c>
       <c r="E147" s="28" t="s">
+        <v>534</v>
+      </c>
+      <c r="F147" s="28" t="s">
         <v>476</v>
       </c>
     </row>
-    <row r="148" spans="1:5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A148" s="28" t="s">
         <v>200</v>
       </c>
-      <c r="B148" s="28" t="s">
+      <c r="C148" s="28" t="s">
         <v>513</v>
       </c>
-      <c r="D148" s="28" t="s">
-        <v>535</v>
-      </c>
       <c r="E148" s="28" t="s">
+        <v>534</v>
+      </c>
+      <c r="F148" s="28" t="s">
         <v>476</v>
       </c>
     </row>
-    <row r="149" spans="1:5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A149" s="28" t="s">
         <v>196</v>
       </c>
-      <c r="B149" s="28" t="s">
-        <v>533</v>
-      </c>
-      <c r="D149" s="28" t="s">
-        <v>535</v>
+      <c r="C149" s="28" t="s">
+        <v>532</v>
       </c>
       <c r="E149" s="28" t="s">
+        <v>534</v>
+      </c>
+      <c r="F149" s="28" t="s">
         <v>476</v>
       </c>
     </row>
-    <row r="150" spans="1:5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A150" s="28" t="s">
         <v>202</v>
       </c>
-      <c r="B150" s="28" t="s">
-        <v>534</v>
-      </c>
-      <c r="D150" s="28" t="s">
+      <c r="C150" s="28" t="s">
+        <v>533</v>
+      </c>
+      <c r="E150" s="28" t="s">
         <v>476</v>
       </c>
     </row>
-    <row r="151" spans="1:5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A151" s="28" t="s">
         <v>188</v>
       </c>
-    </row>
-    <row r="152" spans="1:5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C151" s="28" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="152" spans="1:6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A152" s="28" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="153" spans="1:5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C152" s="28" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="153" spans="1:6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A153" s="28" t="s">
         <v>190</v>
       </c>
-    </row>
-    <row r="154" spans="1:5" ht="55.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C153" s="28" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="154" spans="1:6" ht="55.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A154" s="28" t="s">
         <v>208</v>
       </c>
-      <c r="B154" s="28" t="s">
+      <c r="C154" s="28" t="s">
         <v>408</v>
       </c>
-      <c r="C154" s="29" t="s">
-        <v>553</v>
-      </c>
-      <c r="D154" s="28" t="s">
-        <v>536</v>
+      <c r="D154" s="29" t="s">
+        <v>551</v>
       </c>
       <c r="E154" s="28" t="s">
+        <v>535</v>
+      </c>
+      <c r="F154" s="28" t="s">
         <v>469</v>
       </c>
     </row>
-    <row r="155" spans="1:5" ht="55.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:6" ht="55.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A155" s="28" t="s">
         <v>206</v>
       </c>
-      <c r="B155" s="28" t="s">
-        <v>526</v>
-      </c>
-      <c r="C155" s="29" t="s">
-        <v>554</v>
-      </c>
-      <c r="D155" s="28" t="s">
-        <v>536</v>
+      <c r="C155" s="28" t="s">
+        <v>525</v>
+      </c>
+      <c r="D155" s="29" t="s">
+        <v>552</v>
       </c>
       <c r="E155" s="28" t="s">
+        <v>535</v>
+      </c>
+      <c r="F155" s="28" t="s">
         <v>469</v>
       </c>
     </row>
-    <row r="156" spans="1:5" ht="55.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:6" ht="55.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A156" s="28" t="s">
         <v>210</v>
       </c>
-      <c r="B156" s="28" t="s">
-        <v>523</v>
-      </c>
-      <c r="C156" s="29" t="s">
-        <v>555</v>
-      </c>
-      <c r="D156" s="28" t="s">
-        <v>536</v>
+      <c r="C156" s="28" t="s">
+        <v>522</v>
+      </c>
+      <c r="D156" s="29" t="s">
+        <v>553</v>
       </c>
       <c r="E156" s="28" t="s">
+        <v>535</v>
+      </c>
+      <c r="F156" s="28" t="s">
         <v>469</v>
       </c>
     </row>
-    <row r="157" spans="1:5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A157" s="28" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="158" spans="1:5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A158" s="28" t="s">
         <v>68</v>
       </c>
-      <c r="B158" s="28" t="s">
+      <c r="C158" s="28" t="s">
         <v>463</v>
       </c>
-      <c r="C158" s="29" t="s">
-        <v>546</v>
-      </c>
-      <c r="D158" s="28" t="s">
+      <c r="D158" s="29" t="s">
+        <v>544</v>
+      </c>
+      <c r="E158" s="28" t="s">
         <v>355</v>
       </c>
     </row>
-    <row r="159" spans="1:5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A159" s="28" t="s">
         <v>60</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D163">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F159">
     <sortCondition ref="A1"/>
   </sortState>
-  <conditionalFormatting sqref="F150:XFD150 A150:D150 A1:XFD149 A151:XFD1048576">
-    <cfRule type="expression" dxfId="0" priority="1">
+  <conditionalFormatting sqref="G150:XFD150 E112:XFD112 E85:XFD85 D150:E150 D151:XFD1048576 D113:XFD149 D86:XFD111 D1:XFD12 E13:XFD14 D15:XFD27 E28:XFD29 D30:XFD34 D36:XFD84 E35:XFD35 A1:C1048576">
+    <cfRule type="expression" dxfId="1" priority="1">
       <formula>MOD(ROW()/2,1)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABF03108-B62E-4189-A7F3-410EEC41743F}">
+  <dimension ref="A1:D159"/>
+  <sheetViews>
+    <sheetView topLeftCell="A88" workbookViewId="0">
+      <selection activeCell="B101" sqref="A1:D1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" thickBottom="1" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="37.88671875" style="28" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.33203125" style="28" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.5546875" style="28" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.109375" style="28" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="27" t="s">
+        <v>315</v>
+      </c>
+      <c r="B1" s="27" t="s">
+        <v>519</v>
+      </c>
+      <c r="C1" s="27" t="s">
+        <v>521</v>
+      </c>
+      <c r="D1" s="27"/>
+    </row>
+    <row r="2" spans="1:4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="28" t="s">
+        <v>54</v>
+      </c>
+      <c r="B2" s="28" t="s">
+        <v>325</v>
+      </c>
+      <c r="C2" s="28" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="28" t="s">
+        <v>113</v>
+      </c>
+      <c r="B3" s="28" t="s">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="28" t="s">
+        <v>213</v>
+      </c>
+      <c r="B4" s="28" t="s">
+        <v>575</v>
+      </c>
+      <c r="C4" s="28" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="28" t="s">
+        <v>89</v>
+      </c>
+      <c r="B5" s="28" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="28" t="s">
+        <v>219</v>
+      </c>
+      <c r="B6" s="28" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="28" t="s">
+        <v>204</v>
+      </c>
+      <c r="B7" s="28" t="s">
+        <v>530</v>
+      </c>
+      <c r="C7" s="28" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="28" t="s">
+        <v>34</v>
+      </c>
+      <c r="B8" s="28" t="s">
+        <v>426</v>
+      </c>
+      <c r="C8" s="28" t="s">
+        <v>565</v>
+      </c>
+      <c r="D8" s="28" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="28" t="s">
+        <v>217</v>
+      </c>
+      <c r="B9" s="28" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="28" t="s">
+        <v>111</v>
+      </c>
+      <c r="B10" s="28" t="s">
+        <v>554</v>
+      </c>
+      <c r="C10" s="28" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="28" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" s="28" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="28" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" s="28" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="28" t="s">
+        <v>212</v>
+      </c>
+      <c r="B13" s="28" t="s">
+        <v>362</v>
+      </c>
+      <c r="C13" s="28" t="s">
+        <v>569</v>
+      </c>
+      <c r="D13" s="28" t="s">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="28" t="s">
+        <v>28</v>
+      </c>
+      <c r="B14" s="28" t="s">
+        <v>362</v>
+      </c>
+      <c r="C14" s="28" t="s">
+        <v>363</v>
+      </c>
+      <c r="D14" s="28" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="28" t="s">
+        <v>239</v>
+      </c>
+      <c r="B15" s="28" t="s">
+        <v>362</v>
+      </c>
+      <c r="C15" s="28" t="s">
+        <v>578</v>
+      </c>
+      <c r="D15" s="28" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="28" t="s">
+        <v>26</v>
+      </c>
+      <c r="B16" s="28" t="s">
+        <v>362</v>
+      </c>
+      <c r="C16" s="28" t="s">
+        <v>367</v>
+      </c>
+      <c r="D16" s="28" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="28" t="s">
+        <v>103</v>
+      </c>
+      <c r="B17" s="28" t="s">
+        <v>362</v>
+      </c>
+      <c r="C17" s="28" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="28" t="s">
+        <v>194</v>
+      </c>
+      <c r="B18" s="28" t="s">
+        <v>362</v>
+      </c>
+      <c r="C18" s="28" t="s">
+        <v>534</v>
+      </c>
+      <c r="D18" s="28" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="28" t="s">
+        <v>233</v>
+      </c>
+      <c r="B19" s="28" t="s">
+        <v>365</v>
+      </c>
+      <c r="C19" s="28" t="s">
+        <v>363</v>
+      </c>
+      <c r="D19" s="28" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="28" t="s">
+        <v>235</v>
+      </c>
+      <c r="B20" s="28" t="s">
+        <v>365</v>
+      </c>
+      <c r="C20" s="28" t="s">
+        <v>367</v>
+      </c>
+      <c r="D20" s="28" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="28" t="s">
+        <v>84</v>
+      </c>
+      <c r="B21" s="28" t="s">
+        <v>520</v>
+      </c>
+      <c r="C21" s="28" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="28" t="s">
+        <v>32</v>
+      </c>
+      <c r="B22" s="28" t="s">
+        <v>520</v>
+      </c>
+      <c r="C22" s="28" t="s">
+        <v>542</v>
+      </c>
+      <c r="D22" s="28" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="28" t="s">
+        <v>6</v>
+      </c>
+      <c r="B23" s="28" t="s">
+        <v>520</v>
+      </c>
+      <c r="C23" s="28" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="28" t="s">
+        <v>166</v>
+      </c>
+      <c r="B24" s="28" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="28" t="s">
+        <v>86</v>
+      </c>
+      <c r="B25" s="28" t="s">
+        <v>484</v>
+      </c>
+      <c r="C25" s="28" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="28" t="s">
+        <v>172</v>
+      </c>
+      <c r="B26" s="28" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="28" t="s">
+        <v>170</v>
+      </c>
+      <c r="B27" s="28" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="B28" s="28" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="28" t="s">
+        <v>174</v>
+      </c>
+      <c r="B29" s="28" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="B30" s="28" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="28" t="s">
+        <v>176</v>
+      </c>
+      <c r="B31" s="28" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A32" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="B32" s="28" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A33" s="28" t="s">
+        <v>178</v>
+      </c>
+      <c r="B33" s="28" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A34" s="28" t="s">
+        <v>180</v>
+      </c>
+      <c r="B34" s="28" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A35" s="28" t="s">
+        <v>182</v>
+      </c>
+      <c r="B35" s="28" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A36" s="28" t="s">
+        <v>184</v>
+      </c>
+      <c r="B36" s="28" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A37" s="28" t="s">
+        <v>168</v>
+      </c>
+      <c r="B37" s="28" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A38" s="28" t="s">
+        <v>186</v>
+      </c>
+      <c r="B38" s="28" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A39" s="28" t="s">
+        <v>93</v>
+      </c>
+      <c r="B39" s="28" t="s">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A40" s="28" t="s">
+        <v>20</v>
+      </c>
+      <c r="B40" s="28" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A41" s="28" t="s">
+        <v>137</v>
+      </c>
+      <c r="B41" s="28" t="s">
+        <v>564</v>
+      </c>
+      <c r="C41" s="28" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A42" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="B42" s="28" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A43" s="28" t="s">
+        <v>146</v>
+      </c>
+      <c r="B43" s="28" t="s">
+        <v>396</v>
+      </c>
+      <c r="C43" s="28" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A44" s="28" t="s">
+        <v>18</v>
+      </c>
+      <c r="B44" s="28" t="s">
+        <v>499</v>
+      </c>
+      <c r="C44" s="28" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A45" s="28" t="s">
+        <v>16</v>
+      </c>
+      <c r="B45" s="28" t="s">
+        <v>499</v>
+      </c>
+      <c r="C45" s="28" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A46" s="28" t="s">
+        <v>109</v>
+      </c>
+      <c r="B46" s="28" t="s">
+        <v>558</v>
+      </c>
+      <c r="C46" s="28" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A47" s="28" t="s">
+        <v>105</v>
+      </c>
+      <c r="B47" s="28" t="s">
+        <v>454</v>
+      </c>
+      <c r="C47" s="28" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A48" s="28" t="s">
+        <v>0</v>
+      </c>
+      <c r="B48" s="28" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A49" s="28" t="s">
+        <v>208</v>
+      </c>
+      <c r="B49" s="28" t="s">
+        <v>408</v>
+      </c>
+      <c r="C49" s="28" t="s">
+        <v>535</v>
+      </c>
+      <c r="D49" s="28" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A50" s="28" t="s">
+        <v>247</v>
+      </c>
+      <c r="B50" s="28" t="s">
+        <v>579</v>
+      </c>
+      <c r="C50" s="28" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A51" s="28" t="s">
+        <v>243</v>
+      </c>
+      <c r="B51" s="28" t="s">
+        <v>577</v>
+      </c>
+      <c r="C51" s="28" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A52" s="28" t="s">
+        <v>305</v>
+      </c>
+      <c r="B52" s="28" t="s">
+        <v>413</v>
+      </c>
+      <c r="C52" s="28" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A53" s="28" t="s">
+        <v>99</v>
+      </c>
+      <c r="B53" s="28" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A54" s="28" t="s">
+        <v>135</v>
+      </c>
+      <c r="B54" s="28" t="s">
+        <v>524</v>
+      </c>
+      <c r="C54" s="28" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A55" s="28" t="s">
+        <v>107</v>
+      </c>
+      <c r="B55" s="28" t="s">
+        <v>524</v>
+      </c>
+      <c r="C55" s="28" t="s">
+        <v>513</v>
+      </c>
+      <c r="D55" s="28" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A56" s="28" t="s">
+        <v>101</v>
+      </c>
+      <c r="B56" s="28" t="s">
+        <v>524</v>
+      </c>
+      <c r="C56" s="28" t="s">
+        <v>549</v>
+      </c>
+      <c r="D56" s="28" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A57" s="28" t="s">
+        <v>133</v>
+      </c>
+      <c r="B57" s="28" t="s">
+        <v>524</v>
+      </c>
+      <c r="C57" s="28" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A58" s="28" t="s">
+        <v>198</v>
+      </c>
+      <c r="B58" s="28" t="s">
+        <v>524</v>
+      </c>
+      <c r="C58" s="28" t="s">
+        <v>534</v>
+      </c>
+      <c r="D58" s="28" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A59" s="28" t="s">
+        <v>97</v>
+      </c>
+      <c r="B59" s="28" t="s">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A60" s="28" t="s">
+        <v>253</v>
+      </c>
+      <c r="B60" s="28" t="s">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A61" s="28" t="s">
+        <v>200</v>
+      </c>
+      <c r="B61" s="28" t="s">
+        <v>513</v>
+      </c>
+      <c r="C61" s="28" t="s">
+        <v>534</v>
+      </c>
+      <c r="D61" s="28" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A62" s="28" t="s">
+        <v>95</v>
+      </c>
+      <c r="B62" s="28" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A63" s="28" t="s">
+        <v>62</v>
+      </c>
+      <c r="B63" s="28" t="s">
+        <v>546</v>
+      </c>
+      <c r="C63" s="28" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A64" s="28" t="s">
+        <v>66</v>
+      </c>
+      <c r="B64" s="28" t="s">
+        <v>546</v>
+      </c>
+      <c r="C64" s="28" t="s">
+        <v>559</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A65" s="28" t="s">
+        <v>64</v>
+      </c>
+      <c r="B65" s="28" t="s">
+        <v>546</v>
+      </c>
+      <c r="C65" s="28" t="s">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A66" s="28" t="s">
+        <v>8</v>
+      </c>
+      <c r="B66" s="28" t="s">
+        <v>543</v>
+      </c>
+      <c r="C66" s="28" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A67" s="28" t="s">
+        <v>148</v>
+      </c>
+      <c r="B67" s="28" t="s">
+        <v>435</v>
+      </c>
+      <c r="C67" s="28" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A68" s="28" t="s">
+        <v>196</v>
+      </c>
+      <c r="B68" s="28" t="s">
+        <v>532</v>
+      </c>
+      <c r="C68" s="28" t="s">
+        <v>534</v>
+      </c>
+      <c r="D68" s="28" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A69" s="28" t="s">
+        <v>131</v>
+      </c>
+      <c r="B69" s="28" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A70" s="28" t="s">
+        <v>221</v>
+      </c>
+      <c r="B70" s="28" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A71" s="28" t="s">
+        <v>129</v>
+      </c>
+      <c r="B71" s="28" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A72" s="28" t="s">
+        <v>202</v>
+      </c>
+      <c r="B72" s="28" t="s">
+        <v>533</v>
+      </c>
+      <c r="C72" s="28" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A73" s="28" t="s">
+        <v>50</v>
+      </c>
+      <c r="B73" s="28" t="s">
+        <v>443</v>
+      </c>
+      <c r="C73" s="28" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A74" s="28" t="s">
+        <v>52</v>
+      </c>
+      <c r="B74" s="28" t="s">
+        <v>493</v>
+      </c>
+      <c r="C74" s="28" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A75" s="28" t="s">
+        <v>251</v>
+      </c>
+      <c r="B75" s="28" t="s">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A76" s="28" t="s">
+        <v>2</v>
+      </c>
+      <c r="B76" s="28" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A77" s="28" t="s">
+        <v>206</v>
+      </c>
+      <c r="B77" s="28" t="s">
+        <v>525</v>
+      </c>
+      <c r="C77" s="28" t="s">
+        <v>535</v>
+      </c>
+      <c r="D77" s="28" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A78" s="28" t="s">
+        <v>152</v>
+      </c>
+      <c r="B78" s="28" t="s">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A79" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="B79" s="28" t="s">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A80" s="28" t="s">
+        <v>210</v>
+      </c>
+      <c r="B80" s="28" t="s">
+        <v>522</v>
+      </c>
+      <c r="C80" s="28" t="s">
+        <v>535</v>
+      </c>
+      <c r="D80" s="28" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A81" s="28" t="s">
+        <v>154</v>
+      </c>
+      <c r="B81" s="28" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A82" s="28" t="s">
+        <v>156</v>
+      </c>
+      <c r="B82" s="28" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A83" s="28" t="s">
+        <v>158</v>
+      </c>
+      <c r="B83" s="28" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A84" s="28" t="s">
+        <v>160</v>
+      </c>
+      <c r="B84" s="28" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A85" s="28" t="s">
+        <v>72</v>
+      </c>
+      <c r="B85" s="28" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A86" s="28" t="s">
+        <v>56</v>
+      </c>
+      <c r="B86" s="28" t="s">
+        <v>449</v>
+      </c>
+      <c r="C86" s="28" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A87" s="28" t="s">
+        <v>144</v>
+      </c>
+      <c r="B87" s="28" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A88" s="28" t="s">
+        <v>30</v>
+      </c>
+      <c r="B88" s="28" t="s">
+        <v>529</v>
+      </c>
+      <c r="C88" s="28" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A89" s="28" t="s">
+        <v>91</v>
+      </c>
+      <c r="B89" s="28" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A90" s="28" t="s">
+        <v>140</v>
+      </c>
+      <c r="B90" s="28" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A91" s="28" t="s">
+        <v>87</v>
+      </c>
+      <c r="B91" s="28" t="s">
+        <v>39</v>
+      </c>
+      <c r="C91" s="28" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A92" s="28" t="s">
+        <v>38</v>
+      </c>
+      <c r="B92" s="28" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A93" s="28" t="s">
+        <v>42</v>
+      </c>
+      <c r="B93" s="28" t="s">
+        <v>479</v>
+      </c>
+      <c r="C93" s="28" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A94" s="28" t="s">
+        <v>249</v>
+      </c>
+      <c r="B94" s="28" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A95" s="28" t="s">
+        <v>255</v>
+      </c>
+      <c r="B95" s="28" t="s">
+        <v>452</v>
+      </c>
+      <c r="C95" s="28" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A96" s="28" t="s">
+        <v>257</v>
+      </c>
+      <c r="B96" s="28" t="s">
+        <v>452</v>
+      </c>
+      <c r="C96" s="28" t="s">
+        <v>574</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A97" s="28" t="s">
+        <v>188</v>
+      </c>
+      <c r="B97" s="28" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A98" s="28" t="s">
+        <v>192</v>
+      </c>
+      <c r="B98" s="28" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A99" s="28" t="s">
+        <v>190</v>
+      </c>
+      <c r="B99" s="28" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A100" s="28" t="s">
+        <v>241</v>
+      </c>
+      <c r="B100" s="28" t="s">
+        <v>580</v>
+      </c>
+      <c r="C100" s="28" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A101" s="28" t="s">
+        <v>68</v>
+      </c>
+      <c r="B101" s="28" t="s">
+        <v>463</v>
+      </c>
+      <c r="C101" s="28" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A102" s="28" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A103" s="28" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A104" s="28" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A105" s="28" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A106" s="28" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A107" s="28" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A108" s="28" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A109" s="28" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A110" s="28" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A111" s="28" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A112" s="28" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="113" spans="1:1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A113" s="28" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="114" spans="1:1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A114" s="28" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="115" spans="1:1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A115" s="28" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="116" spans="1:1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A116" s="28" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="117" spans="1:1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A117" s="28" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="118" spans="1:1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A118" s="28" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="119" spans="1:1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A119" s="28" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="120" spans="1:1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A120" s="28" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="121" spans="1:1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A121" s="28" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="122" spans="1:1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A122" s="28" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="123" spans="1:1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A123" s="28" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="124" spans="1:1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A124" s="28" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="125" spans="1:1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A125" s="28" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="126" spans="1:1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A126" s="28" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="127" spans="1:1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A127" s="28" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="128" spans="1:1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A128" s="28" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="129" spans="1:1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A129" s="28" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="130" spans="1:1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A130" s="28" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="131" spans="1:1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A131" s="28" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="132" spans="1:1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A132" s="28" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="133" spans="1:1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A133" s="28" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="134" spans="1:1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A134" s="28" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="135" spans="1:1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A135" s="28" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="136" spans="1:1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A136" s="28" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="137" spans="1:1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A137" s="28" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="138" spans="1:1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A138" s="28" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="139" spans="1:1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A139" s="28" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="140" spans="1:1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A140" s="28" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="141" spans="1:1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A141" s="28" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="142" spans="1:1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A142" s="28" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="143" spans="1:1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A143" s="28" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="144" spans="1:1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A144" s="28" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="145" spans="1:1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A145" s="28" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="146" spans="1:1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A146" s="28" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="147" spans="1:1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A147" s="28" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="148" spans="1:1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A148" s="28" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="149" spans="1:1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A149" s="28" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="150" spans="1:1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A150" s="28" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="151" spans="1:1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A151" s="28" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="152" spans="1:1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A152" s="28" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="153" spans="1:1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A153" s="28" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="154" spans="1:1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A154" s="28" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="155" spans="1:1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A155" s="28" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="156" spans="1:1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A156" s="28" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="157" spans="1:1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A157" s="28" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="158" spans="1:1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A158" s="28" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="159" spans="1:1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A159" s="28" t="s">
+        <v>60</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="D151:D1048576 D1:D149 A1:C1048576">
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>MOD(ROW()/2,1)&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
v0.3, _hash, _mal_ref, value --> data
</commit_message>
<xml_diff>
--- a/Attributes and Objects Documentation.xlsx
+++ b/Attributes and Objects Documentation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\tahoe\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C282DB23-ABBD-462C-8180-72B65B8986D3}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C2EE2D6-DE05-4F19-BDB9-BA8F45DD90DC}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{11D50969-177D-481F-A7AD-9647F67FC210}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{11D50969-177D-481F-A7AD-9647F67FC210}"/>
   </bookViews>
   <sheets>
     <sheet name="misp" sheetId="3" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1344" uniqueCount="680">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1344" uniqueCount="679">
   <si>
     <t xml:space="preserve">md5 </t>
   </si>
@@ -2064,9 +2064,6 @@
   </si>
   <si>
     <t>network_traffic</t>
-  </si>
-  <si>
-    <t>ssh_login</t>
   </si>
   <si>
     <t>login.success</t>
@@ -2743,9 +2740,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FD3A4BA-035A-49B6-AE8D-CE931CE2DC31}">
   <dimension ref="A1:F159"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A117" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B1" sqref="A1:B1048576"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A115" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B122" sqref="B122"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" thickBottom="1" x14ac:dyDescent="0.35"/>
@@ -3730,7 +3727,7 @@
         <v>442</v>
       </c>
       <c r="D112" s="29" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
     </row>
     <row r="113" spans="1:5" thickBot="1" x14ac:dyDescent="0.35">
@@ -3845,7 +3842,7 @@
         <v>446</v>
       </c>
       <c r="D123" s="29" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="E123" s="28" t="s">
         <v>355</v>
@@ -4189,7 +4186,7 @@
         <v>208</v>
       </c>
       <c r="B154" s="29" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="C154" s="28" t="s">
         <v>408</v>
@@ -4209,7 +4206,7 @@
         <v>206</v>
       </c>
       <c r="B155" s="29" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="C155" s="28" t="s">
         <v>525</v>
@@ -4226,10 +4223,10 @@
     </row>
     <row r="156" spans="1:6" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A156" s="28" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="B156" s="29" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="C156" s="28" t="s">
         <v>522</v>
@@ -4286,9 +4283,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABF03108-B62E-4189-A7F3-410EEC41743F}">
   <dimension ref="A1:J47"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D1" sqref="D1:E1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H40" sqref="H40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" thickBottom="1" x14ac:dyDescent="0.3"/>
@@ -4311,13 +4308,13 @@
         <v>627</v>
       </c>
       <c r="B1" s="34" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="C1" s="31" t="s">
         <v>577</v>
       </c>
       <c r="D1" s="34" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="E1" s="31" t="s">
         <v>573</v>
@@ -4329,7 +4326,7 @@
         <v>632</v>
       </c>
       <c r="I1" s="34" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="J1" s="31" t="s">
         <v>340</v>
@@ -4814,7 +4811,7 @@
         <v>638</v>
       </c>
       <c r="J29" s="32" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
     </row>
     <row r="30" spans="1:10" thickBot="1" x14ac:dyDescent="0.3">
@@ -4828,7 +4825,7 @@
         <v>638</v>
       </c>
       <c r="J30" s="32" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
     </row>
     <row r="31" spans="1:10" thickBot="1" x14ac:dyDescent="0.3">
@@ -4941,7 +4938,7 @@
         <v>652</v>
       </c>
       <c r="H37" s="32" t="s">
-        <v>655</v>
+        <v>611</v>
       </c>
     </row>
     <row r="38" spans="1:10" thickBot="1" x14ac:dyDescent="0.3">
@@ -4958,7 +4955,7 @@
         <v>652</v>
       </c>
       <c r="H38" s="32" t="s">
-        <v>655</v>
+        <v>611</v>
       </c>
     </row>
     <row r="39" spans="1:10" thickBot="1" x14ac:dyDescent="0.3">
@@ -4969,62 +4966,62 @@
         <v>640</v>
       </c>
       <c r="H39" s="32" t="s">
-        <v>655</v>
+        <v>611</v>
       </c>
       <c r="J39" s="32" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
     </row>
     <row r="40" spans="1:10" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="32" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="D40" s="32" t="s">
         <v>640</v>
       </c>
       <c r="H40" s="32" t="s">
-        <v>655</v>
+        <v>611</v>
       </c>
       <c r="J40" s="32" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
     </row>
     <row r="41" spans="1:10" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="32" t="s">
+        <v>658</v>
+      </c>
+      <c r="B41" s="33" t="s">
         <v>659</v>
       </c>
-      <c r="B41" s="33" t="s">
-        <v>660</v>
-      </c>
       <c r="I41" s="32" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
     </row>
     <row r="42" spans="1:10" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="32" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="B42" s="32" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="I42" s="32" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
     </row>
     <row r="43" spans="1:10" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="32" t="s">
+        <v>665</v>
+      </c>
+      <c r="B43" s="33" t="s">
         <v>666</v>
       </c>
-      <c r="B43" s="33" t="s">
+      <c r="I43" s="32" t="s">
         <v>667</v>
-      </c>
-      <c r="I43" s="32" t="s">
-        <v>668</v>
       </c>
     </row>
     <row r="44" spans="1:10" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="32" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="B44" s="32" t="s">
         <v>39</v>
@@ -5033,12 +5030,12 @@
         <v>39</v>
       </c>
       <c r="H44" s="32" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
     </row>
     <row r="45" spans="1:10" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="32" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="D45" s="32" t="s">
         <v>520</v>
@@ -5047,18 +5044,18 @@
         <v>374</v>
       </c>
       <c r="H45" s="32" t="s">
+        <v>669</v>
+      </c>
+      <c r="J45" s="32" t="s">
         <v>670</v>
-      </c>
-      <c r="J45" s="32" t="s">
-        <v>671</v>
       </c>
     </row>
     <row r="46" spans="1:10" ht="28.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="32" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="B46" s="32" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="D46" s="32" t="s">
         <v>522</v>
@@ -5070,21 +5067,21 @@
         <v>374</v>
       </c>
       <c r="H46" s="32" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
     </row>
     <row r="47" spans="1:10" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="32" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="D47" s="32" t="s">
         <v>640</v>
       </c>
       <c r="H47" s="32" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="J47" s="32" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
     </row>
   </sheetData>

</xml_diff>